<commit_message>
Created drafts of LogicUnit.vhd and Adder.vhd. The latter is copied from Lab 2
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E3578F-2353-4A44-A42D-D5CB8621B29A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A47C8A4-84C4-46A6-BB36-144CA723BB43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Updated folders as per instructions. Set up ModelSim and Quartus project files</t>
+  </si>
+  <si>
+    <t>Created a draft of LogicUnit.vhd (have not compiled it yet)</t>
+  </si>
+  <si>
+    <t>Copied over Lab 2 into Adder.vhd (have not compiled it yet)</t>
+  </si>
+  <si>
+    <t>Formatted LogicUnit.vhd and Adder.vhd to look nicer</t>
   </si>
 </sst>
 </file>
@@ -626,7 +635,7 @@
   <dimension ref="A1:G756"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,25 +802,55 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="18"/>
-      <c r="G12" s="11"/>
+      <c r="B12" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C12" s="9">
+        <v>43923</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0.46875</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="18"/>
-      <c r="G13" s="11"/>
+      <c r="B13" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C13" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D13" s="16">
+        <v>1</v>
+      </c>
+      <c r="E13" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="18"/>
-      <c r="G14" s="11"/>
+      <c r="B14" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C14" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D14" s="16">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E14" s="18">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>

</xml_diff>

<commit_message>
First attempt at ArithUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A47C8A4-84C4-46A6-BB36-144CA723BB43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2841B14-238B-40F2-A85C-2CE0EA4CA068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Formatted LogicUnit.vhd and Adder.vhd to look nicer</t>
+  </si>
+  <si>
+    <t>Mild symptoms. Will rest and continue work on it next week</t>
+  </si>
+  <si>
+    <t>Started work on Arithmetic Unit. Stopped to look back at notes to fully understand Arithmetic Unit before continueing</t>
   </si>
 </sst>
 </file>
@@ -632,7 +638,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
-  <dimension ref="A1:G756"/>
+  <dimension ref="A1:G757"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
@@ -755,16 +761,16 @@
         <v>6977</v>
       </c>
       <c r="C9" s="9">
-        <v>43923</v>
+        <v>43918</v>
       </c>
       <c r="D9" s="16">
-        <v>0.83888888888888891</v>
+        <v>0.5</v>
       </c>
       <c r="E9" s="18">
-        <v>0.84166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -775,13 +781,13 @@
         <v>43923</v>
       </c>
       <c r="D10" s="16">
-        <v>0.3430555555555555</v>
+        <v>0.83888888888888891</v>
       </c>
       <c r="E10" s="18">
-        <v>0.3444444444444445</v>
+        <v>0.84166666666666667</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -792,13 +798,13 @@
         <v>43923</v>
       </c>
       <c r="D11" s="16">
-        <v>0.8833333333333333</v>
+        <v>0.3430555555555555</v>
       </c>
       <c r="E11" s="18">
-        <v>0.9243055555555556</v>
+        <v>0.3444444444444445</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -809,13 +815,13 @@
         <v>43923</v>
       </c>
       <c r="D12" s="16">
-        <v>0.46875</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="E12" s="18">
-        <v>0</v>
+        <v>0.9243055555555556</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -823,16 +829,16 @@
         <v>6977</v>
       </c>
       <c r="C13" s="9">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="D13" s="16">
-        <v>1</v>
+        <v>0.46875</v>
       </c>
       <c r="E13" s="18">
-        <v>2.0833333333333332E-2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -843,28 +849,48 @@
         <v>43924</v>
       </c>
       <c r="D14" s="16">
+        <v>1</v>
+      </c>
+      <c r="E14" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E14" s="18">
+      <c r="G14" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C15" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D15" s="16">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E15" s="18">
         <v>3.125E-2</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="18"/>
-      <c r="G15" s="11"/>
-    </row>
     <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="18"/>
-      <c r="G16" s="11"/>
+      <c r="B16" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C16" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D16" s="16">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="E16" s="18">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11"/>
@@ -1111,14 +1137,20 @@
       <c r="E51" s="18"/>
       <c r="G51" s="11"/>
     </row>
-    <row r="52" spans="2:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="12"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="19"/>
-      <c r="G52" s="12"/>
-    </row>
-    <row r="53" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="11"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="18"/>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="2:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="12"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="19"/>
+      <c r="G53" s="12"/>
+    </row>
     <row r="54" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1822,6 +1854,7 @@
     <row r="754" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="755" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="756" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
Attempted to compile project on Quartus. Fixed .vhd files as necessary. Included output_files on purpose
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2841B14-238B-40F2-A85C-2CE0EA4CA068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2282C0-F9E7-48C3-BBEA-6B0224E03959}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="28680" yWindow="3555" windowWidth="38640" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -101,7 +101,16 @@
     <t>Mild symptoms. Will rest and continue work on it next week</t>
   </si>
   <si>
-    <t>Started work on Arithmetic Unit. Stopped to look back at notes to fully understand Arithmetic Unit before continueing</t>
+    <t>Started work on ArithUnit.vhd. Stopped to look back at notes to fully understand Arithmetic Unit before continueing</t>
+  </si>
+  <si>
+    <t>Fixing LogicUnit.vhd, Adder.vhd and ArithUnit.vhd to make it compile Quartus. Not done</t>
+  </si>
+  <si>
+    <t>Added .gitignore to ignore some of the Quartus generated files</t>
+  </si>
+  <si>
+    <t>Added .gitignore to ignore Office temporary files. Makes it annoying to accidentally include temporary files to commit</t>
   </si>
 </sst>
 </file>
@@ -641,7 +650,7 @@
   <dimension ref="A1:G757"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,25 +902,55 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="18"/>
-      <c r="G17" s="11"/>
+      <c r="B17" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C17" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D17" s="16">
+        <v>8.4027777777777771E-2</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0.11597222222222221</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="18"/>
-      <c r="G18" s="11"/>
+      <c r="B18" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C18" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D18" s="16">
+        <v>0.11597222222222221</v>
+      </c>
+      <c r="E18" s="18">
+        <v>0.14166666666666666</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="18"/>
-      <c r="G19" s="11"/>
+      <c r="B19" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C19" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0.14166666666666666</v>
+      </c>
+      <c r="E19" s="18">
+        <v>0.14791666666666667</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11"/>

</xml_diff>

<commit_message>
Compiled LogicUnit.vhd and LogicGates.vhd. Changed project settings. Added and renamed files to Documentation folder as per instructions
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A415A2DA-777A-4DC6-BFE1-80C0F732D906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03C14C2-C584-4200-9AB1-2FFFC981555F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="585" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>Updated .gitignore to ignore ModelSim and more Quartus generated files</t>
+  </si>
+  <si>
+    <t>Created LogicGates.vhd to include logic gates for the LogicUnit.vhd. Fixed compilation issues with LogicGates.vhd.</t>
+  </si>
+  <si>
+    <t>Fixed possible compilation issue with Adder.vhd (untested)</t>
+  </si>
+  <si>
+    <t>Compiled LogicUnit.vhd successfully. Renamed files according to PDF document and moved them into Documentation folder</t>
   </si>
 </sst>
 </file>
@@ -652,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G757"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,32 +975,62 @@
         <v>0.83680555555555547</v>
       </c>
       <c r="E20" s="18">
-        <v>0.84097222222222223</v>
+        <v>0.84652777777777777</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="18"/>
-      <c r="G21" s="11"/>
+      <c r="B21" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C21" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D21" s="16">
+        <v>0.85486111111111107</v>
+      </c>
+      <c r="E21" s="18">
+        <v>0.87222222222222223</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="18"/>
-      <c r="G22" s="11"/>
+      <c r="B22" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C22" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D22" s="16">
+        <v>0.87222222222222223</v>
+      </c>
+      <c r="E22" s="18">
+        <v>0.87638888888888899</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="18"/>
-      <c r="G23" s="11"/>
+      <c r="B23" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C23" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D23" s="16">
+        <v>0.87638888888888899</v>
+      </c>
+      <c r="E23" s="18">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>

</xml_diff>

<commit_message>
Added behavioural architecture to ArithUnit.vhd. Compiled on both ModelSim and Quartus
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03C14C2-C584-4200-9AB1-2FFFC981555F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C08A3B-2786-460E-BA4B-09F55C78C201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="585" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>Compiled LogicUnit.vhd successfully. Renamed files according to PDF document and moved them into Documentation folder</t>
+  </si>
+  <si>
+    <t>Fixed folder structure and files as they were incorrect. Fixed project file settings</t>
+  </si>
+  <si>
+    <t>Ran scripts for Test Benches and ConfigExU. Fixed changes along the way (but still does not run successfully)</t>
+  </si>
+  <si>
+    <t>Fixed ArithUnit.vhd and Adder.vhd so they compile on ModelSim and Quartus.</t>
   </si>
 </sst>
 </file>
@@ -662,7 +671,7 @@
   <dimension ref="A1:G757"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,25 +1042,55 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="18"/>
-      <c r="G24" s="11"/>
+      <c r="B24" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C24" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D24" s="16">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="E24" s="18">
+        <v>0.89930555555555547</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="18"/>
-      <c r="G25" s="11"/>
+      <c r="B25" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C25" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D25" s="16">
+        <v>0.89930555555555547</v>
+      </c>
+      <c r="E25" s="18">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="18"/>
-      <c r="G26" s="11"/>
+      <c r="B26" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C26" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D26" s="16">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="E26" s="18">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>

</xml_diff>

<commit_message>
Fixed .vhd files to run .do files. Compiles properly. Configuration .do scripts work now
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C08A3B-2786-460E-BA4B-09F55C78C201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440E64E6-ECEF-44CC-B824-B43A192F24C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="16395" yWindow="2910" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Fixed ArithUnit.vhd and Adder.vhd so they compile on ModelSim and Quartus.</t>
+  </si>
+  <si>
+    <t>Fixed ArithUnit.vhd and Adder.vhd such that both .do scripts work (previosuly they do not work as pointed out by my teammates). Each script works if and only if all ports are defined properly</t>
   </si>
 </sst>
 </file>
@@ -671,7 +674,7 @@
   <dimension ref="A1:G757"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,11 +1096,21 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="18"/>
-      <c r="G27" s="11"/>
+      <c r="B27" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C27" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D27" s="16">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="E27" s="18">
+        <v>0.96875</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>

</xml_diff>

<commit_message>
Configured setup and environment to grab timing simulations for LogicUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440E64E6-ECEF-44CC-B824-B43A192F24C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083C527F-8ACC-4851-989E-7EC96AD21F08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16395" yWindow="2910" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>Fixed ArithUnit.vhd and Adder.vhd such that both .do scripts work (previosuly they do not work as pointed out by my teammates). Each script works if and only if all ports are defined properly</t>
+  </si>
+  <si>
+    <t>Generated the functional waveforms of the LogicUnit.vhd. Exported them into Documentation as per instructions</t>
+  </si>
+  <si>
+    <t>Systhesied circuits but not satisfied with the diagrams due to it being very cluttered. Will grab the images later when a revised version is done</t>
+  </si>
+  <si>
+    <t>Set up files and environment to obtain timing simulations from ModelSim</t>
+  </si>
+  <si>
+    <t>Updated .gitignore to ignore temporary files that is unneeded</t>
   </si>
 </sst>
 </file>
@@ -674,7 +686,7 @@
   <dimension ref="A1:G757"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,32 +1125,72 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="18"/>
-      <c r="G28" s="11"/>
+      <c r="B28" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C28" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D28" s="16">
+        <v>0.96875</v>
+      </c>
+      <c r="E28" s="18">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="29" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="18"/>
-      <c r="G29" s="11"/>
+      <c r="B29" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C29" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D29" s="16">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E29" s="18">
+        <v>0.99652777777777779</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="30" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="18"/>
-      <c r="G30" s="11"/>
+      <c r="B30" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C30" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D30" s="16">
+        <v>0.99652777777777779</v>
+      </c>
+      <c r="E30" s="18">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="18"/>
-      <c r="G31" s="11"/>
+      <c r="B31" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C31" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D31" s="16">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="E31" s="18">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="32" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11"/>

</xml_diff>

<commit_message>
Generated timing waveforms for LogicUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083C527F-8ACC-4851-989E-7EC96AD21F08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B1B0C0-619B-4905-9704-E9D19E2D0F77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Updated .gitignore to ignore temporary files that is unneeded</t>
+  </si>
+  <si>
+    <t>Obtained timing waveforms and added them to Documentation as per instructions.</t>
   </si>
 </sst>
 </file>
@@ -685,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,11 +1196,21 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="18"/>
-      <c r="G32" s="11"/>
+      <c r="B32" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C32" s="9">
+        <v>43924</v>
+      </c>
+      <c r="D32" s="16">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="E32" s="18">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="33" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11"/>

</xml_diff>

<commit_message>
Updated functional waveforms for LogicUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B1B0C0-619B-4905-9704-E9D19E2D0F77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05D155F-EB5B-4E90-A147-B60F4848CED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>Obtained timing waveforms and added them to Documentation as per instructions.</t>
+  </si>
+  <si>
+    <t>Added TestVectors. Discovered a bug in LogicUnit.vhd. Stopped for dinner</t>
+  </si>
+  <si>
+    <t>Fixed LogicUnit.vhd.</t>
+  </si>
+  <si>
+    <t>Updated Functional Waveforms.</t>
   </si>
 </sst>
 </file>
@@ -688,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1192,7 @@
         <v>6977</v>
       </c>
       <c r="C31" s="9">
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="D31" s="16">
         <v>3.472222222222222E-3</v>
@@ -1200,7 +1209,7 @@
         <v>6977</v>
       </c>
       <c r="C32" s="9">
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="D32" s="16">
         <v>8.3333333333333332E-3</v>
@@ -1213,28 +1222,60 @@
       </c>
     </row>
     <row r="33" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="18"/>
-      <c r="G33" s="11"/>
+      <c r="B33" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C33" s="9">
+        <v>43925</v>
+      </c>
+      <c r="D33" s="16">
+        <v>0.7090277777777777</v>
+      </c>
+      <c r="E33" s="18">
+        <v>0.75763888888888886</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="34" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="18"/>
-      <c r="G34" s="11"/>
+      <c r="B34" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C34" s="9">
+        <v>43925</v>
+      </c>
+      <c r="D34" s="16">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="E34" s="18">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="35" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="11"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="18"/>
-      <c r="G35" s="11"/>
+      <c r="B35" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C35" s="9">
+        <v>43925</v>
+      </c>
+      <c r="D35" s="16">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="E35" s="18">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="36" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
+      <c r="B36" s="11">
+        <v>6977</v>
+      </c>
       <c r="C36" s="9"/>
       <c r="D36" s="16"/>
       <c r="E36" s="18"/>

</xml_diff>

<commit_message>
Updated timing waveforms for LogicUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05D155F-EB5B-4E90-A147-B60F4848CED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4919386F-8214-47B8-BF07-E3BEF2136870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -158,7 +158,13 @@
     <t>Fixed LogicUnit.vhd.</t>
   </si>
   <si>
-    <t>Updated Functional Waveforms.</t>
+    <t>Created RTL netlist images and Post-fit images</t>
+  </si>
+  <si>
+    <t>Updated Timing waveforms for LogicUnit.vhd</t>
+  </si>
+  <si>
+    <t>Updated Functional Waveforms for LogicUnit.vhd</t>
   </si>
 </sst>
 </file>
@@ -698,7 +704,7 @@
   <dimension ref="A1:G757"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,24 +1275,42 @@
         <v>0.94791666666666663</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
         <v>6977</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="18"/>
-      <c r="G36" s="11"/>
+      <c r="C36" s="9">
+        <v>43925</v>
+      </c>
+      <c r="D36" s="16">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="E36" s="18">
+        <v>0.96180555555555547</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="37" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="11"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="18"/>
-      <c r="G37" s="11"/>
+      <c r="B37" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C37" s="9">
+        <v>43925</v>
+      </c>
+      <c r="D37" s="16">
+        <v>0.96180555555555547</v>
+      </c>
+      <c r="E37" s="18">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="38" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>

</xml_diff>

<commit_message>
Rearranged Documentation strucutre. Updated report to add in truth table and block diagram of LogicUnit
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4919386F-8214-47B8-BF07-E3BEF2136870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4DCF0D-13DB-456E-A176-7B9D7C84036B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Updated Functional Waveforms for LogicUnit.vhd</t>
+  </si>
+  <si>
+    <t>Updated folder structure of Documentation directory. Started working on the report.</t>
   </si>
 </sst>
 </file>
@@ -704,7 +707,7 @@
   <dimension ref="A1:G757"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,11 +1316,21 @@
       </c>
     </row>
     <row r="38" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="11"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="18"/>
-      <c r="G38" s="11"/>
+      <c r="B38" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C38" s="9">
+        <v>43925</v>
+      </c>
+      <c r="D38" s="16">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E38" s="18">
+        <v>0.98749999999999993</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="39" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="11"/>

</xml_diff>

<commit_message>
Updated document. Fixed bug in LogicUnit.vhd.
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4DCF0D-13DB-456E-A176-7B9D7C84036B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50A9381-3059-446B-89E2-AF977ECCE69A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Updated folder structure of Documentation directory. Started working on the report.</t>
+  </si>
+  <si>
+    <t>Added overview sections of LogicUnit to report. Noticed that Truth table documented is different than VHDL code</t>
+  </si>
+  <si>
+    <t>Re-compiled VHDL code. Reproduced all diagrams to match documentation</t>
   </si>
 </sst>
 </file>
@@ -707,7 +713,7 @@
   <dimension ref="A1:G757"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,18 +1339,36 @@
       </c>
     </row>
     <row r="39" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="11"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="18"/>
-      <c r="G39" s="11"/>
+      <c r="B39" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C39" s="9">
+        <v>43925</v>
+      </c>
+      <c r="D39" s="16">
+        <v>0.98749999999999993</v>
+      </c>
+      <c r="E39" s="18">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="40" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="11"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="16"/>
+      <c r="B40" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C40" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D40" s="16">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="E40" s="18"/>
-      <c r="G40" s="11"/>
+      <c r="G40" s="11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="41" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="11"/>

</xml_diff>

<commit_message>
Updated Functional Simulation Diagrams for LogicUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50A9381-3059-446B-89E2-AF977ECCE69A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A145E7E-952C-457D-99C1-CBE8BDF1A725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -173,7 +173,7 @@
     <t>Added overview sections of LogicUnit to report. Noticed that Truth table documented is different than VHDL code</t>
   </si>
   <si>
-    <t>Re-compiled VHDL code. Reproduced all diagrams to match documentation</t>
+    <t>Re-compiled VHDL code</t>
   </si>
 </sst>
 </file>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,17 +1365,29 @@
       <c r="D40" s="16">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="E40" s="18"/>
+      <c r="E40" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G40" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="18"/>
-      <c r="G41" s="11"/>
+      <c r="B41" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C41" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D41" s="16">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E41" s="18">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="42" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>

</xml_diff>

<commit_message>
Renamed .vho and .sdo files for LogicUnit. Exported .vho, .sdo, .map.summary and .fit.summary files to Documentation folder of LogicUnit
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A145E7E-952C-457D-99C1-CBE8BDF1A725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE5867A-CCEB-4119-9C02-DFD4F188DD74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Re-compiled VHDL code</t>
+  </si>
+  <si>
+    <t>Renamed .vho and .sdo files for LogicUnit. Exported .vho, .sdo, .map.summary and .fit.summary files to Documentation folder of LogicUnit</t>
   </si>
 </sst>
 </file>
@@ -712,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G45" sqref="A44:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,11 +1393,21 @@
       </c>
     </row>
     <row r="42" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="11"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="18"/>
-      <c r="G42" s="11"/>
+      <c r="B42" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C42" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D42" s="16">
+        <v>0.53611111111111109</v>
+      </c>
+      <c r="E42" s="18">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="43" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11"/>

</xml_diff>

<commit_message>
Added waveforms to document
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E0A9D6-48F6-4B89-AF9E-FDC06BD5DA7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B918C8-C311-44FC-A320-955ADCDBFB4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Renamed .vho and .sdo files for LogicUnit. Exported .vho, .sdo, .map.summary and .fit.summary files to Documentation folder of LogicUnit</t>
+  </si>
+  <si>
+    <t>Added waveforms for LogicUnit.vhd to document</t>
   </si>
 </sst>
 </file>
@@ -716,7 +719,7 @@
   <dimension ref="A1:G757"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,11 +1430,21 @@
       </c>
     </row>
     <row r="44" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="18"/>
-      <c r="G44" s="11"/>
+      <c r="B44" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C44" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D44" s="16">
+        <v>6.8749999999999992E-2</v>
+      </c>
+      <c r="E44" s="18">
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="45" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="11"/>

</xml_diff>